<commit_message>
fixed some syntax bugs
</commit_message>
<xml_diff>
--- a/Methods description.xlsx
+++ b/Methods description.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="71">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -68,133 +68,136 @@
     <t xml:space="preserve">Operator +</t>
   </si>
   <si>
+    <t xml:space="preserve">BigInt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">adding two BigInts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Truờng</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Operator – (2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">subtracting two BigInts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Operator – (1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Opposite operator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Operator *</t>
+  </si>
+  <si>
+    <t xml:space="preserve">multiplying two BigInts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Operator /</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dividing two BigInts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Operator !</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Return 0 if nonzero, else 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bảo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Operator ~</t>
+  </si>
+  <si>
+    <t xml:space="preserve">flipping bits</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Operator &amp;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bitwise and</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Operator |</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bitwise or</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Operator ^</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bitwise exclusive-or (xor)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Operator &lt;&lt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">left shifting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Operator &gt;&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">right shifting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">arithmetic shifting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Operator ==</t>
+  </si>
+  <si>
+    <t xml:space="preserve">true/false</t>
+  </si>
+  <si>
+    <t xml:space="preserve">equal comparison</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Operator !=</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not-equal comparison</t>
+  </si>
+  <si>
+    <t xml:space="preserve">may reuse opt ==</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Operator &lt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Less-than comparison</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Operator &gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Greater-than comparison</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Operator &lt;=</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Less-than-or-equal comparison</t>
+  </si>
+  <si>
+    <t xml:space="preserve">may reuse opt &gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Operator &gt;=</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Greater-than-or-equal comparison</t>
+  </si>
+  <si>
+    <t xml:space="preserve">may reuse opt &lt;</t>
+  </si>
+  <si>
     <t xml:space="preserve">BigNum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">adding two BigInts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Truờng</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Operator – (2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">subtracting two BigInts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Operator – (1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Opposite operator</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Operator *</t>
-  </si>
-  <si>
-    <t xml:space="preserve">multiplying two BigInts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Operator /</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dividing two BigInts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Operator !</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Return 0 if nonzero, else 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bảo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Operator ~</t>
-  </si>
-  <si>
-    <t xml:space="preserve">flipping bits</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Operator &amp;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bitwise and</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Operator |</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bitwise or</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Operator ^</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bitwise exclusive-or (xor)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Operator &lt;&lt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">left shifting</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Operator &gt;&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">right shifting</t>
-  </si>
-  <si>
-    <t xml:space="preserve">arithmetic shifting</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Operator ==</t>
-  </si>
-  <si>
-    <t xml:space="preserve">true/false</t>
-  </si>
-  <si>
-    <t xml:space="preserve">equal comparison</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Operator !=</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Not-equal comparison</t>
-  </si>
-  <si>
-    <t xml:space="preserve">may reuse opt ==</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Operator &lt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Less-than comparison</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Operator &gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Greater-than comparison</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Operator &lt;=</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Less-than-or-equal comparison</t>
-  </si>
-  <si>
-    <t xml:space="preserve">may reuse opt &gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Operator &gt;=</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Greater-than-or-equal comparison</t>
-  </si>
-  <si>
-    <t xml:space="preserve">may reuse opt &lt;</t>
   </si>
   <si>
     <t xml:space="preserve">Default constructor</t>
@@ -356,7 +359,7 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E21" activeCellId="0" sqref="E21:E22"/>
+      <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -443,7 +446,7 @@
       <c r="A6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="0" t="s">
         <v>15</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -471,7 +474,7 @@
       <c r="A8" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="0" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="2" t="s">
@@ -485,7 +488,7 @@
       <c r="A9" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="0" t="s">
         <v>15</v>
       </c>
       <c r="C9" s="2" t="s">
@@ -576,7 +579,7 @@
         <v>38</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -593,7 +596,7 @@
         <v>41</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -702,7 +705,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F6" activeCellId="1" sqref="E21:E22 F6"/>
+      <selection pane="topLeft" activeCell="F6" activeCellId="1" sqref="E16 F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -735,13 +738,13 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>15</v>
+        <v>58</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E2" s="0" t="s">
         <v>17</v>
@@ -749,7 +752,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>8</v>
@@ -760,13 +763,13 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E4" s="0" t="s">
         <v>17</v>
@@ -774,13 +777,13 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E5" s="0" t="s">
         <v>17</v>
@@ -788,13 +791,13 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E6" s="0" t="s">
         <v>17</v>

</xml_diff>